<commit_message>
Added camera list searching and sorting tests
</commit_message>
<xml_diff>
--- a/test_data/example.xlsx
+++ b/test_data/example.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -28,7 +28,7 @@
     <t xml:space="preserve">Name</t>
   </si>
   <si>
-    <t xml:space="preserve">6.3</t>
+    <t xml:space="preserve">5.3</t>
   </si>
   <si>
     <t xml:space="preserve">UNDEFINED</t>
@@ -55,10 +55,7 @@
     <t xml:space="preserve">кабинет 1-ЭТ</t>
   </si>
   <si>
-    <t xml:space="preserve">None</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Camera</t>
+    <t xml:space="preserve">NaN</t>
   </si>
 </sst>
 </file>
@@ -144,7 +141,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -166,6 +163,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -189,7 +190,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -212,7 +213,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -259,12 +260,8 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
-        <v>109</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>12</v>
-      </c>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>